<commit_message>
Cambio en la lista de usuarios
</commit_message>
<xml_diff>
--- a/Usuarios.xlsx
+++ b/Usuarios.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luisa\Videos\Estatica\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32BF8D74-3B6A-4CFD-A69E-8052F7C19A42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F70BA78D-FC43-421C-83BC-BED124C9A1C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5FCB3F99-0261-46C5-A7DB-000A3E5FEA35}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>a.amayad@uniandes.edu.co</t>
   </si>
@@ -98,9 +98,6 @@
     <t>l.lora@uniandes.edu.co</t>
   </si>
   <si>
-    <t>d.lusic@uniandes.edu.co</t>
-  </si>
-  <si>
     <t>sd.martinezm1@uniandes.edu.co</t>
   </si>
   <si>
@@ -159,13 +156,46 @@
   </si>
   <si>
     <t>password</t>
+  </si>
+  <si>
+    <t>e.ruedab@uniandes.edu.co</t>
+  </si>
+  <si>
+    <t>202113919</t>
+  </si>
+  <si>
+    <t>msanchez</t>
+  </si>
+  <si>
+    <t>j.echeverriaz@uniandes.edu.co</t>
+  </si>
+  <si>
+    <t>l.camargob@uniandes.edu.co</t>
+  </si>
+  <si>
+    <t>ja.pacheco2@uniandes.edu.co</t>
+  </si>
+  <si>
+    <t>202110979</t>
+  </si>
+  <si>
+    <t>202225307</t>
+  </si>
+  <si>
+    <t>202312291</t>
+  </si>
+  <si>
+    <t>ms.moreno@uniandes.edu.co</t>
+  </si>
+  <si>
+    <t>ms.moreno</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,14 +208,6 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -205,22 +227,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -553,346 +574,384 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97F4342E-D3FF-408C-9030-D6794B723DC6}">
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.21875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" style="2"/>
-    <col min="3" max="16384" width="11.5546875" style="1"/>
+    <col min="1" max="1" width="32.5546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>40</v>
-      </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>37</v>
+      <c r="A2" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="B2" s="4">
         <v>201621920</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" s="4">
-        <v>20240826</v>
+      <c r="A3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="4">
+      <c r="B8" s="3">
         <v>202311076</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B9" s="3">
         <v>202324690</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B10" s="3">
         <v>202216289</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B11" s="3">
         <v>202223500</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B12" s="3">
         <v>202316240</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B13" s="3">
         <v>202113581</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B14" s="3">
         <v>202310071</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B15" s="3">
         <v>202226904</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B16" s="3">
         <v>202210777</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B17" s="3">
         <v>202323451</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B18" s="3">
         <v>202325527</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="4">
+      <c r="B19" s="3">
         <v>202021167</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B20" s="3">
         <v>202011069</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B17" s="4">
+      <c r="B21" s="3">
         <v>202320909</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="4">
+      <c r="B22" s="3">
         <v>202315124</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="4">
+      <c r="B23" s="3">
         <v>202310600</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="4">
+      <c r="B24" s="3">
         <v>202211008</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="4">
+      <c r="B25" s="3">
         <v>202320961</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="4">
+      <c r="B26" s="3">
         <v>202311071</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="4">
+      <c r="B27" s="3">
         <v>202221005</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="4">
-        <v>202424811</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
+      <c r="B28" s="3">
+        <v>202310123</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B25" s="4">
-        <v>202310123</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
+      <c r="B29" s="3">
+        <v>202310131</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="4">
-        <v>202310131</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
+      <c r="B30" s="3">
+        <v>202320183</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B27" s="4">
-        <v>202320183</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
+      <c r="B31" s="3">
+        <v>202321062</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B28" s="4">
-        <v>202321062</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
+      <c r="B32" s="3">
+        <v>202214571</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B29" s="4">
-        <v>202214571</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
+      <c r="B33" s="3">
+        <v>202321098</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B30" s="4">
-        <v>202321098</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
+      <c r="B34" s="3">
+        <v>202311745</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="4">
-        <v>202311745</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
+      <c r="B35" s="3">
+        <v>202112458</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B32" s="4">
-        <v>202112458</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
+      <c r="B36" s="3">
+        <v>202321180</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B33" s="4">
-        <v>202321180</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
+      <c r="B37" s="3">
+        <v>202310864</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B34" s="4">
-        <v>202310864</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
+      <c r="B38" s="3">
+        <v>202112796</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B35" s="4">
-        <v>202112796</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
+      <c r="B40" s="3">
+        <v>201915258</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="4">
-        <v>201915258</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="3" t="s">
+      <c r="B41" s="3">
+        <v>202323882</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B37" s="4">
-        <v>202323882</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
+      <c r="B42" s="3">
+        <v>202313312</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B38" s="4">
-        <v>202313312</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="3" t="s">
+      <c r="B43" s="3">
+        <v>202321378</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B39" s="4">
-        <v>202321378</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B40" s="4">
+      <c r="B44" s="3">
         <v>202312447</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A33" r:id="rId1" display="mailto:ja.palacios@uniandes.edu.co" xr:uid="{576F1019-FDBF-4705-AA32-886CD89B1C9C}"/>
-    <hyperlink ref="A13" r:id="rId2" xr:uid="{8930BA18-E3A7-4FC3-9223-1E2222513BF8}"/>
-    <hyperlink ref="A19" r:id="rId3" xr:uid="{89C8CEA6-6B55-45B1-912C-8DD7FDF224F8}"/>
+    <hyperlink ref="A36" r:id="rId1" display="mailto:ja.palacios@uniandes.edu.co" xr:uid="{576F1019-FDBF-4705-AA32-886CD89B1C9C}"/>
+    <hyperlink ref="A17" r:id="rId2" xr:uid="{8930BA18-E3A7-4FC3-9223-1E2222513BF8}"/>
+    <hyperlink ref="A23" r:id="rId3" xr:uid="{89C8CEA6-6B55-45B1-912C-8DD7FDF224F8}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{87D77BEE-CC1A-4D77-B094-42827A4325C5}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{89ABD2BF-D12D-4620-A392-61EE626014CC}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{FB0D0346-C19B-4E5C-8BE3-583F4E777E3C}"/>
+    <hyperlink ref="A4" r:id="rId7" xr:uid="{BCD113FD-972E-4ABA-8122-49F9F1F4D090}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
+  <ignoredErrors>
+    <ignoredError sqref="B5:B7 B39" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>